<commit_message>
improved rule description handling
</commit_message>
<xml_diff>
--- a/resources/OntoUML Rules.xlsx
+++ b/resources/OntoUML Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FavatoBarcelosPP\Dev\ontouml-validator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA43FFD-8E68-4D37-A338-20182A5B8AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A019468-DD42-4025-BD09-D981676755CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="401">
   <si>
     <t>Description</t>
   </si>
@@ -826,9 +826,6 @@
     <t>SQU</t>
   </si>
   <si>
-    <t>ANJ</t>
-  </si>
-  <si>
     <t>JMQ</t>
   </si>
   <si>
@@ -1087,9 +1084,6 @@
     <t>abstract, datatype, enumeration</t>
   </si>
   <si>
-    <t>Every class decorated with an stereotype in the ABSTRACT LIST must have the tagged value "restrictedTo" set to an array containing the value [ "abstract" ].</t>
-  </si>
-  <si>
     <t>No generalization can connect a general class decorated with a sortal stereotype to a specific class decorated with a non-sortal stereotype.</t>
   </si>
   <si>
@@ -1120,9 +1114,6 @@
     <t>mixin</t>
   </si>
   <si>
-    <t>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, and situation to situation.</t>
-  </si>
-  <si>
     <t>Stereotype not set without tagged value</t>
   </si>
   <si>
@@ -1223,6 +1214,30 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</t>
+  </si>
+  <si>
+    <t>R_CL_EMV</t>
+  </si>
+  <si>
+    <t>Stereotype without tagged value</t>
+  </si>
+  <si>
+    <t>Stereotype with single valid tagged value</t>
+  </si>
+  <si>
+    <t>Stereotype with two valid tagged values</t>
+  </si>
+  <si>
+    <t>Stereotype with two invalid tagged values</t>
+  </si>
+  <si>
+    <t>Stereotype with one valid and one invalid tagged values</t>
+  </si>
+  <si>
+    <t>Stereotype with single invalid tagged value</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1375,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1405,55 +1420,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1481,36 +1454,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1759,62 +1702,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}" name="TabRules" displayName="TabRules" ref="A1:D71" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:D71" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D71">
-    <sortCondition ref="A2:A71"/>
-    <sortCondition ref="D2:D71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}" name="TabRules" displayName="TabRules" ref="A1:D70" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:D70" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D70">
+    <sortCondition ref="A2:A70"/>
+    <sortCondition ref="D2:D70"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F9D36F48-DD19-43E5-A1AB-8357F96419FF}" name="Group" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{050EF7A6-273B-408D-B0A1-784D6DF4A5AB}" name="ID" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{05F466FD-E5DB-4DED-979E-C9E29087B8F6}" name="Rule Code" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{F9D36F48-DD19-43E5-A1AB-8357F96419FF}" name="Group" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{050EF7A6-273B-408D-B0A1-784D6DF4A5AB}" name="ID" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{05F466FD-E5DB-4DED-979E-C9E29087B8F6}" name="Rule Code" dataDxfId="20">
       <calculatedColumnFormula>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{70BA6684-6E4A-40D9-BE42-830C46F4D6A9}" name="Description" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{70BA6684-6E4A-40D9-BE42-830C46F4D6A9}" name="Description" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D8A1ADE-544A-443A-AF20-52BBCA41FA15}" name="TabGroups" displayName="TabGroups" ref="F1:G6" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D8A1ADE-544A-443A-AF20-52BBCA41FA15}" name="TabGroups" displayName="TabGroups" ref="F1:G6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="F1:G6" xr:uid="{3D8A1ADE-544A-443A-AF20-52BBCA41FA15}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2E543EF0-9E26-4478-A5D0-A70AC90899EE}" name="Group" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{2A3CE154-AB6B-45C3-B5E2-2E1AC49C63C7}" name="Group Code" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{2E543EF0-9E26-4478-A5D0-A70AC90899EE}" name="Group" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{2A3CE154-AB6B-45C3-B5E2-2E1AC49C63C7}" name="Group Code" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}" name="TabImp" displayName="TabImp" ref="A1:K119" totalsRowShown="0">
-  <autoFilter ref="A1:K119" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}" name="TabImp" displayName="TabImp" ref="A1:K127" totalsRowShown="0">
+  <autoFilter ref="A1:K127" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K93">
     <sortCondition ref="A1:A93"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5662254C-D4AB-4E75-B315-CAFCAA30EDF4}" name="Rule Code" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{65D02219-A7C8-4BC4-BE70-FC12D26642C7}" name="Rule Description" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{5662254C-D4AB-4E75-B315-CAFCAA30EDF4}" name="Rule Code" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{65D02219-A7C8-4BC4-BE70-FC12D26642C7}" name="Rule Description" dataDxfId="13">
       <calculatedColumnFormula>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{39BF0221-09C6-4746-A9C6-D71D4B6C7533}" name="Situation"/>
-    <tableColumn id="6" xr3:uid="{FE3246A6-E21A-441F-A08A-12268F822A02}" name="Situation Code" dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{FE3246A6-E21A-441F-A08A-12268F822A02}" name="Situation Code" dataDxfId="12">
       <calculatedColumnFormula>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ED1E7C03-7BE4-4AD0-867B-6CF8D46CE033}" name="Test File" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{ED1E7C03-7BE4-4AD0-867B-6CF8D46CE033}" name="Test File" dataDxfId="11">
       <calculatedColumnFormula>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{F491E82A-09B4-4B22-AA08-7E6DFD336A64}" name="Situation Description"/>
     <tableColumn id="4" xr3:uid="{92BCF063-80EB-4A9C-AA1A-6F95CC9435A7}" name="OWA Level"/>
-    <tableColumn id="7" xr3:uid="{DB4F2106-6953-489A-AB24-1163C09441FE}" name="CWA Level" dataDxfId="17">
+    <tableColumn id="7" xr3:uid="{DB4F2106-6953-489A-AB24-1163C09441FE}" name="CWA Level" dataDxfId="10">
       <calculatedColumnFormula>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E91C3898-466B-4A4C-8CF6-E0B90D5094B2}" name="Test OWA Entry" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{E91C3898-466B-4A4C-8CF6-E0B90D5094B2}" name="Test OWA Entry" dataDxfId="9">
       <calculatedColumnFormula>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D99049E8-95AA-440A-B6C3-AB032C08C4B8}" name="Test CWA Entry" dataDxfId="15">
+    <tableColumn id="11" xr3:uid="{D99049E8-95AA-440A-B6C3-AB032C08C4B8}" name="Test CWA Entry" dataDxfId="8">
       <calculatedColumnFormula>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{9CF1643D-B8F2-452E-B29E-AD6EF72070C4}" name="Comments"/>
@@ -1830,7 +1773,7 @@
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D8098905-7B35-4419-9FF0-ABB475A5357D}" name="Stereotype List" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{D8098905-7B35-4419-9FF0-ABB475A5357D}" name="Stereotype List" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{F12CB8CE-6969-4083-9729-E8A90699DB57}" name="Stereotypes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2137,12 +2080,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G95" sqref="G95"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2295,7 +2238,7 @@
         <v>R_CL_LAX</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7"/>
@@ -2312,7 +2255,7 @@
         <v>R_CL_ZGT</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2327,7 +2270,7 @@
         <v>R_CL_ASZ</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2342,7 +2285,7 @@
         <v>R_CL_YOK</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2357,7 +2300,7 @@
         <v>R_CL_QJC</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>361</v>
+        <v>393</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>244</v>
@@ -2413,14 +2356,14 @@
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="C15" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_ANJ</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>350</v>
+        <v>R_CL_XJZ</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2428,14 +2371,14 @@
         <v>1</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C16" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_XJZ</v>
+        <v>R_CL_JOJ</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2443,14 +2386,14 @@
         <v>1</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C17" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_JOJ</v>
+        <v>R_CL_GJU</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2458,14 +2401,14 @@
         <v>1</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C18" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_GJU</v>
+        <v>R_CL_BWZ</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2473,14 +2416,14 @@
         <v>1</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C19" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_BWZ</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>2</v>
+        <v>R_CL_JMQ</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2492,10 +2435,10 @@
       </c>
       <c r="C20" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_JMQ</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>14</v>
+        <v>R_CL_EMV</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2507,10 +2450,10 @@
       </c>
       <c r="C21" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_EMV</v>
+        <v>R_CL_QOV</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>9</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2522,10 +2465,10 @@
       </c>
       <c r="C22" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_QOV</v>
+        <v>R_CL_JFW</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>357</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2537,10 +2480,10 @@
       </c>
       <c r="C23" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_JFW</v>
+        <v>R_CL_UTL</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2552,10 +2495,10 @@
       </c>
       <c r="C24" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_UTL</v>
+        <v>R_CL_VPE</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2567,10 +2510,10 @@
       </c>
       <c r="C25" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_VPE</v>
+        <v>R_CL_BFO</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2582,10 +2525,10 @@
       </c>
       <c r="C26" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_BFO</v>
+        <v>R_CL_VOQ</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2597,10 +2540,10 @@
       </c>
       <c r="C27" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_VOQ</v>
+        <v>R_CL_GAZ</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2612,10 +2555,10 @@
       </c>
       <c r="C28" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_GAZ</v>
+        <v>R_CL_BQI</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2623,14 +2566,14 @@
         <v>1</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="C29" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_BQI</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>7</v>
+        <v>R_CL_UMC</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2638,14 +2581,14 @@
         <v>1</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="C30" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_UMC</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>98</v>
+        <v>R_CL_OEV</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2657,10 +2600,10 @@
       </c>
       <c r="C31" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_OEV</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>20</v>
+        <v>R_CL_EGT</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2672,25 +2615,25 @@
       </c>
       <c r="C32" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_EGT</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>377</v>
+        <v>R_CL_ANY</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>276</v>
       </c>
       <c r="C33" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_ANY</v>
+        <v>R_GE_XRS</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2702,10 +2645,10 @@
       </c>
       <c r="C34" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_XRS</v>
+        <v>R_GE_MDR</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2717,10 +2660,10 @@
       </c>
       <c r="C35" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_MDR</v>
+        <v>R_GE_BAK</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2732,10 +2675,10 @@
       </c>
       <c r="C36" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_BAK</v>
+        <v>R_GE_JLW</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2747,10 +2690,10 @@
       </c>
       <c r="C37" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_JLW</v>
+        <v>R_GE_VEZ</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2762,10 +2705,10 @@
       </c>
       <c r="C38" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_VEZ</v>
+        <v>R_GE_IJM</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2777,10 +2720,10 @@
       </c>
       <c r="C39" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_IJM</v>
+        <v>R_GE_UXR</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2792,10 +2735,10 @@
       </c>
       <c r="C40" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_UXR</v>
+        <v>R_GE_HGQ</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>23</v>
+        <v>349</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2807,10 +2750,10 @@
       </c>
       <c r="C41" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_HGQ</v>
+        <v>R_GE_EPG</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2822,10 +2765,10 @@
       </c>
       <c r="C42" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_EPG</v>
+        <v>R_GE_MXI</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>338</v>
+        <v>356</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2837,25 +2780,25 @@
       </c>
       <c r="C43" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_MXI</v>
+        <v>R_GE_HPZ</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>358</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>287</v>
       </c>
       <c r="C44" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_HPZ</v>
+        <v>R_GS_LHD</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2867,10 +2810,10 @@
       </c>
       <c r="C45" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_LHD</v>
+        <v>R_GS_PQP</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2882,10 +2825,10 @@
       </c>
       <c r="C46" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_PQP</v>
+        <v>R_GS_UTW</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2897,10 +2840,10 @@
       </c>
       <c r="C47" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_UTW</v>
+        <v>R_GS_YKW</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2912,10 +2855,10 @@
       </c>
       <c r="C48" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_YKW</v>
+        <v>R_GS_XXB</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2927,25 +2870,25 @@
       </c>
       <c r="C49" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_XXB</v>
+        <v>R_GS_ZMQ</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>293</v>
       </c>
       <c r="C50" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_ZMQ</v>
+        <v>R_PR_BWY</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2957,25 +2900,25 @@
       </c>
       <c r="C51" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_PR_BWY</v>
+        <v>R_PR_LCI</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>295</v>
       </c>
       <c r="C52" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_PR_LCI</v>
+        <v>R_RE_AZO</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2987,10 +2930,10 @@
       </c>
       <c r="C53" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_AZO</v>
+        <v>R_RE_ECP</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3002,10 +2945,10 @@
       </c>
       <c r="C54" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_ECP</v>
+        <v>R_RE_FIX</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3017,10 +2960,10 @@
       </c>
       <c r="C55" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_FIX</v>
+        <v>R_RE_HGG</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3032,10 +2975,10 @@
       </c>
       <c r="C56" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_HGG</v>
+        <v>R_RE_VDQ</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3047,10 +2990,10 @@
       </c>
       <c r="C57" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_VDQ</v>
+        <v>R_RE_VMI</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3062,10 +3005,10 @@
       </c>
       <c r="C58" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_VMI</v>
+        <v>R_RE_ALR</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3077,10 +3020,10 @@
       </c>
       <c r="C59" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_ALR</v>
+        <v>R_RE_SEI</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3092,10 +3035,10 @@
       </c>
       <c r="C60" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_SEI</v>
+        <v>R_RE_EAQ</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3107,10 +3050,10 @@
       </c>
       <c r="C61" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_EAQ</v>
+        <v>R_RE_CDJ</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3122,10 +3065,10 @@
       </c>
       <c r="C62" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_CDJ</v>
+        <v>R_RE_RON</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3137,10 +3080,10 @@
       </c>
       <c r="C63" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_RON</v>
+        <v>R_RE_KZC</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3152,10 +3095,10 @@
       </c>
       <c r="C64" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_KZC</v>
+        <v>R_RE_NTY</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3167,10 +3110,10 @@
       </c>
       <c r="C65" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_NTY</v>
+        <v>R_RE_UCH</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3182,10 +3125,10 @@
       </c>
       <c r="C66" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_UCH</v>
+        <v>R_RE_LQF</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3197,10 +3140,10 @@
       </c>
       <c r="C67" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_LQF</v>
+        <v>R_RE_GZN</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3212,10 +3155,10 @@
       </c>
       <c r="C68" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_GZN</v>
+        <v>R_RE_KPG</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3227,10 +3170,10 @@
       </c>
       <c r="C69" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_KPG</v>
+        <v>R_RE_GZF</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3242,57 +3185,42 @@
       </c>
       <c r="C70" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_GZF</v>
+        <v>R_RE_JND</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="C71" s="9" t="str">
-        <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_JND</v>
-      </c>
-      <c r="D71" s="8" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="5" t="s">
-        <v>60</v>
+      <c r="D73" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D74" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D77" s="11" t="s">
-        <v>337</v>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="11" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B71">
-    <cfRule type="duplicateValues" dxfId="2" priority="38"/>
+  <conditionalFormatting sqref="B2:B70">
+    <cfRule type="duplicateValues" dxfId="6" priority="43"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C71">
-    <cfRule type="duplicateValues" dxfId="1" priority="40"/>
+  <conditionalFormatting sqref="C2:C70">
+    <cfRule type="duplicateValues" dxfId="5" priority="45"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D71">
-    <cfRule type="duplicateValues" dxfId="0" priority="42"/>
+  <conditionalFormatting sqref="D2:D70">
+    <cfRule type="duplicateValues" dxfId="4" priority="47"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3308,11 +3236,11 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:M119"/>
+  <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C109" sqref="C109"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,7 +3266,7 @@
         <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D1" t="s">
         <v>70</v>
@@ -3367,7 +3295,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B2" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3405,7 +3333,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B3" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3443,7 +3371,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B4" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3481,7 +3409,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3519,7 +3447,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3557,7 +3485,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3595,7 +3523,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3633,7 +3561,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B9" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3674,7 +3602,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3715,7 +3643,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B11" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3756,7 +3684,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B12" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3794,7 +3722,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3832,7 +3760,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B14" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3870,7 +3798,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B15" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3908,7 +3836,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B16" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3946,7 +3874,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -3984,7 +3912,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4022,7 +3950,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4063,7 +3991,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4104,7 +4032,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4145,7 +4073,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4183,7 +4111,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4224,7 +4152,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B24" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4265,7 +4193,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B25" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4306,7 +4234,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B26" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4344,7 +4272,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B27" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4382,7 +4310,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B28" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4420,7 +4348,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B29" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4458,7 +4386,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B30" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4496,7 +4424,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B31" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4534,7 +4462,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B32" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4572,7 +4500,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B33" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4610,7 +4538,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B34" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4648,7 +4576,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B35" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4686,7 +4614,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B36" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4724,7 +4652,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B37" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4769,7 +4697,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B38" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4814,7 +4742,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B39" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4859,7 +4787,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B40" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4904,7 +4832,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B41" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4949,7 +4877,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B42" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -4994,7 +4922,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B43" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5039,7 +4967,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B44" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5084,7 +5012,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B45" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5129,7 +5057,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B46" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5174,7 +5102,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B47" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5219,7 +5147,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B48" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5264,7 +5192,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B49" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5309,7 +5237,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B50" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5354,7 +5282,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B51" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5399,7 +5327,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B52" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5444,7 +5372,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B53" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5489,7 +5417,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B54" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5534,7 +5462,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B55" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5579,7 +5507,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B56" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5624,7 +5552,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B57" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5669,7 +5597,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B58" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5714,7 +5642,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B59" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5759,7 +5687,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B60" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5804,7 +5732,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B61" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5849,7 +5777,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B62" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5894,7 +5822,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B63" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5939,7 +5867,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B64" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -5984,7 +5912,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B65" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6029,7 +5957,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B66" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6074,7 +6002,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B67" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6119,7 +6047,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B68" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6164,7 +6092,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B69" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6209,7 +6137,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B70" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6254,7 +6182,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B71" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6299,7 +6227,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B72" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6344,7 +6272,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B73" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6389,7 +6317,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B74" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6434,7 +6362,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B75" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6479,7 +6407,7 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B76" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6524,7 +6452,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B77" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6569,7 +6497,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B78" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6614,7 +6542,7 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B79" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6659,7 +6587,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B80" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6704,7 +6632,7 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B81" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6749,7 +6677,7 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B82" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6794,7 +6722,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B83" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6839,7 +6767,7 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B84" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6884,7 +6812,7 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B85" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6929,7 +6857,7 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B86" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -6974,7 +6902,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B87" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7019,7 +6947,7 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B88" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7064,7 +6992,7 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B89" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7109,7 +7037,7 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B90" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7154,7 +7082,7 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B91" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7199,7 +7127,7 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B92" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7244,7 +7172,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B93" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7289,7 +7217,7 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B94" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7307,7 +7235,7 @@
         <v>R_CL_YOK_A.ttl</v>
       </c>
       <c r="F94" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G94" t="s">
         <v>78</v>
@@ -7327,7 +7255,7 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B95" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7345,7 +7273,7 @@
         <v>R_CL_YOK_B.ttl</v>
       </c>
       <c r="F95" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G95" t="s">
         <v>78</v>
@@ -7365,7 +7293,7 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B96" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7383,7 +7311,7 @@
         <v>R_CL_YOK_C.ttl</v>
       </c>
       <c r="F96" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G96" t="s">
         <v>78</v>
@@ -7401,12 +7329,12 @@
         <v>cwa,R_CL_YOK,R_CL_YOK_C.ttl,valid</v>
       </c>
       <c r="K96" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B97" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7424,7 +7352,7 @@
         <v>R_CL_YOK_D.ttl</v>
       </c>
       <c r="F97" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G97" t="s">
         <v>78</v>
@@ -7442,12 +7370,12 @@
         <v>cwa,R_CL_YOK,R_CL_YOK_D.ttl,valid</v>
       </c>
       <c r="K97" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B98" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7465,7 +7393,7 @@
         <v>R_CL_YOK_E.ttl</v>
       </c>
       <c r="F98" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G98" t="s">
         <v>73</v>
@@ -7483,12 +7411,12 @@
         <v>cwa,R_CL_YOK,R_CL_YOK_E.ttl,error</v>
       </c>
       <c r="K98" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B99" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7506,7 +7434,7 @@
         <v>R_CL_YOK_F.ttl</v>
       </c>
       <c r="F99" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G99" t="s">
         <v>78</v>
@@ -7524,16 +7452,16 @@
         <v>cwa,R_CL_YOK,R_CL_YOK_F.ttl,valid</v>
       </c>
       <c r="K99" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B100" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, and situation to situation.</v>
+        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C100" t="s">
         <v>76</v>
@@ -7547,7 +7475,7 @@
         <v>R_CL_QJC_A.ttl</v>
       </c>
       <c r="F100" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G100" t="s">
         <v>78</v>
@@ -7567,11 +7495,11 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B101" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, and situation to situation.</v>
+        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C101" t="s">
         <v>77</v>
@@ -7585,7 +7513,7 @@
         <v>R_CL_QJC_B.ttl</v>
       </c>
       <c r="F101" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G101" t="s">
         <v>78</v>
@@ -7605,11 +7533,11 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B102" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, and situation to situation.</v>
+        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C102" t="s">
         <v>79</v>
@@ -7623,7 +7551,7 @@
         <v>R_CL_QJC_C.ttl</v>
       </c>
       <c r="F102" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G102" t="s">
         <v>78</v>
@@ -7641,16 +7569,16 @@
         <v>cwa,R_CL_QJC,R_CL_QJC_C.ttl,valid</v>
       </c>
       <c r="K102" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B103" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, and situation to situation.</v>
+        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C103" t="s">
         <v>85</v>
@@ -7664,7 +7592,7 @@
         <v>R_CL_QJC_D.ttl</v>
       </c>
       <c r="F103" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="G103" t="s">
         <v>78</v>
@@ -7682,16 +7610,16 @@
         <v>cwa,R_CL_QJC,R_CL_QJC_D.ttl,valid</v>
       </c>
       <c r="K103" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B104" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, and situation to situation.</v>
+        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C104" t="s">
         <v>86</v>
@@ -7705,34 +7633,34 @@
         <v>R_CL_QJC_E.ttl</v>
       </c>
       <c r="F104" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G104" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H104" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
-        <v>Error</v>
+        <v>Valid</v>
       </c>
       <c r="I104" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
-        <v>owa,R_CL_QJC,R_CL_QJC_E.ttl,warning</v>
+        <v>owa,R_CL_QJC,R_CL_QJC_E.ttl,valid</v>
       </c>
       <c r="J104" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
-        <v>cwa,R_CL_QJC,R_CL_QJC_E.ttl,error</v>
+        <v>cwa,R_CL_QJC,R_CL_QJC_E.ttl,valid</v>
       </c>
       <c r="K104" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B105" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, and situation to situation.</v>
+        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C105" t="s">
         <v>87</v>
@@ -7746,7 +7674,7 @@
         <v>R_CL_QJC_F.ttl</v>
       </c>
       <c r="F105" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G105" t="s">
         <v>73</v>
@@ -7764,19 +7692,19 @@
         <v>cwa,R_CL_QJC,R_CL_QJC_F.ttl,error</v>
       </c>
       <c r="K105" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B106" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, and situation to situation.</v>
+        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C106" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D106" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -7787,7 +7715,7 @@
         <v>R_CL_QJC_G.ttl</v>
       </c>
       <c r="F106" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G106" t="s">
         <v>78</v>
@@ -7805,19 +7733,19 @@
         <v>cwa,R_CL_QJC,R_CL_QJC_G.ttl,valid</v>
       </c>
       <c r="K106" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B107" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, and situation to situation.</v>
+        <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C107" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D107" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -7828,7 +7756,7 @@
         <v>R_CL_QJC_H.ttl</v>
       </c>
       <c r="F107" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G107" t="s">
         <v>73</v>
@@ -7846,501 +7774,805 @@
         <v>cwa,R_CL_QJC,R_CL_QJC_H.ttl,error</v>
       </c>
       <c r="K107" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B108" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B108" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C108" t="s">
         <v>76</v>
       </c>
-      <c r="D108" s="19" t="str">
+      <c r="D108" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_A</v>
       </c>
-      <c r="E108" s="18" t="str">
+      <c r="E108" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_A.ttl</v>
       </c>
       <c r="F108" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="G108" t="s">
         <v>78</v>
       </c>
-      <c r="H108" s="18" t="str">
+      <c r="H108" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Valid</v>
       </c>
-      <c r="I108" s="18" t="str">
+      <c r="I108" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_A.ttl,valid</v>
       </c>
-      <c r="J108" s="18" t="str">
+      <c r="J108" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_A.ttl,valid</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B109" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B109" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C109" t="s">
         <v>77</v>
       </c>
-      <c r="D109" s="19" t="str">
+      <c r="D109" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_B</v>
       </c>
-      <c r="E109" s="18" t="str">
+      <c r="E109" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_B.ttl</v>
       </c>
       <c r="F109" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G109" t="s">
         <v>73</v>
       </c>
-      <c r="H109" s="18" t="str">
+      <c r="H109" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Error</v>
       </c>
-      <c r="I109" s="18" t="str">
+      <c r="I109" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_B.ttl,error</v>
       </c>
-      <c r="J109" s="18" t="str">
+      <c r="J109" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_B.ttl,error</v>
       </c>
       <c r="K109" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B110" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B110" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C110" t="s">
         <v>79</v>
       </c>
-      <c r="D110" s="19" t="str">
+      <c r="D110" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_C</v>
       </c>
-      <c r="E110" s="18" t="str">
+      <c r="E110" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_C.ttl</v>
       </c>
       <c r="F110" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G110" t="s">
         <v>78</v>
       </c>
-      <c r="H110" s="18" t="str">
+      <c r="H110" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Valid</v>
       </c>
-      <c r="I110" s="18" t="str">
+      <c r="I110" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_C.ttl,valid</v>
       </c>
-      <c r="J110" s="18" t="str">
+      <c r="J110" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_C.ttl,valid</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B111" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B111" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C111" t="s">
         <v>85</v>
       </c>
-      <c r="D111" s="19" t="str">
+      <c r="D111" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_D</v>
       </c>
-      <c r="E111" s="18" t="str">
+      <c r="E111" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_D.ttl</v>
       </c>
       <c r="F111" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G111" t="s">
         <v>73</v>
       </c>
-      <c r="H111" s="18" t="str">
+      <c r="H111" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Error</v>
       </c>
-      <c r="I111" s="18" t="str">
+      <c r="I111" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_D.ttl,error</v>
       </c>
-      <c r="J111" s="18" t="str">
+      <c r="J111" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_D.ttl,error</v>
       </c>
       <c r="K111" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B112" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B112" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C112" t="s">
         <v>86</v>
       </c>
-      <c r="D112" s="19" t="str">
+      <c r="D112" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_E</v>
       </c>
-      <c r="E112" s="18" t="str">
+      <c r="E112" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_E.ttl</v>
       </c>
       <c r="F112" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G112" t="s">
         <v>78</v>
       </c>
-      <c r="H112" s="18" t="str">
+      <c r="H112" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Valid</v>
       </c>
-      <c r="I112" s="18" t="str">
+      <c r="I112" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_E.ttl,valid</v>
       </c>
-      <c r="J112" s="18" t="str">
+      <c r="J112" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_E.ttl,valid</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B113" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B113" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C113" t="s">
         <v>87</v>
       </c>
-      <c r="D113" s="19" t="str">
+      <c r="D113" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_F</v>
       </c>
-      <c r="E113" s="18" t="str">
+      <c r="E113" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_F.ttl</v>
       </c>
       <c r="F113" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G113" t="s">
         <v>73</v>
       </c>
-      <c r="H113" s="18" t="str">
+      <c r="H113" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Error</v>
       </c>
-      <c r="I113" s="18" t="str">
+      <c r="I113" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_F.ttl,error</v>
       </c>
-      <c r="J113" s="18" t="str">
+      <c r="J113" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_F.ttl,error</v>
       </c>
       <c r="K113" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B114" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B114" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C114" t="s">
-        <v>370</v>
-      </c>
-      <c r="D114" s="19" t="str">
+        <v>367</v>
+      </c>
+      <c r="D114" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_G</v>
       </c>
-      <c r="E114" s="18" t="str">
+      <c r="E114" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_G.ttl</v>
       </c>
       <c r="F114" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G114" t="s">
         <v>73</v>
       </c>
-      <c r="H114" s="18" t="str">
+      <c r="H114" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Error</v>
       </c>
-      <c r="I114" s="18" t="str">
+      <c r="I114" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_G.ttl,error</v>
       </c>
-      <c r="J114" s="18" t="str">
+      <c r="J114" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_G.ttl,error</v>
       </c>
       <c r="K114" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B115" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B115" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C115" t="s">
-        <v>371</v>
-      </c>
-      <c r="D115" s="19" t="str">
+        <v>368</v>
+      </c>
+      <c r="D115" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_H</v>
       </c>
-      <c r="E115" s="18" t="str">
+      <c r="E115" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_H.ttl</v>
       </c>
       <c r="F115" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G115" t="s">
         <v>78</v>
       </c>
-      <c r="H115" s="18" t="str">
+      <c r="H115" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Valid</v>
       </c>
-      <c r="I115" s="18" t="str">
+      <c r="I115" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_H.ttl,valid</v>
       </c>
-      <c r="J115" s="18" t="str">
+      <c r="J115" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_H.ttl,valid</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B116" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B116" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C116" t="s">
-        <v>391</v>
-      </c>
-      <c r="D116" s="19" t="str">
+        <v>388</v>
+      </c>
+      <c r="D116" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_I</v>
       </c>
-      <c r="E116" s="18" t="str">
+      <c r="E116" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_I.ttl</v>
       </c>
       <c r="F116" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G116" t="s">
         <v>73</v>
       </c>
-      <c r="H116" s="18" t="str">
+      <c r="H116" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Error</v>
       </c>
-      <c r="I116" s="18" t="str">
+      <c r="I116" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_I.ttl,error</v>
       </c>
-      <c r="J116" s="18" t="str">
+      <c r="J116" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_I.ttl,error</v>
       </c>
       <c r="K116" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B117" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B117" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C117" t="s">
-        <v>392</v>
-      </c>
-      <c r="D117" s="19" t="str">
+        <v>389</v>
+      </c>
+      <c r="D117" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_J</v>
       </c>
-      <c r="E117" s="18" t="str">
+      <c r="E117" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_J.ttl</v>
       </c>
       <c r="F117" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G117" t="s">
         <v>73</v>
       </c>
-      <c r="H117" s="18" t="str">
+      <c r="H117" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Error</v>
       </c>
-      <c r="I117" s="18" t="str">
+      <c r="I117" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_J.ttl,error</v>
       </c>
-      <c r="J117" s="18" t="str">
+      <c r="J117" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_J.ttl,error</v>
       </c>
       <c r="K117" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B118" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B118" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C118" t="s">
-        <v>393</v>
-      </c>
-      <c r="D118" s="19" t="str">
+        <v>390</v>
+      </c>
+      <c r="D118" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_K</v>
       </c>
-      <c r="E118" s="18" t="str">
+      <c r="E118" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_K.ttl</v>
       </c>
       <c r="F118" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G118" t="s">
         <v>78</v>
       </c>
-      <c r="H118" s="18" t="str">
+      <c r="H118" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Valid</v>
       </c>
-      <c r="I118" s="18" t="str">
+      <c r="I118" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_K.ttl,valid</v>
       </c>
-      <c r="J118" s="18" t="str">
+      <c r="J118" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_K.ttl,valid</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B119" s="18" t="str">
+        <v>375</v>
+      </c>
+      <c r="B119" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C119" t="s">
-        <v>395</v>
-      </c>
-      <c r="D119" s="19" t="str">
+        <v>392</v>
+      </c>
+      <c r="D119" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
         <v>R_CL_EGT_L</v>
       </c>
-      <c r="E119" s="18" t="str">
+      <c r="E119" t="str">
         <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
         <v>R_CL_EGT_L.ttl</v>
       </c>
       <c r="F119" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G119" t="s">
         <v>73</v>
       </c>
-      <c r="H119" s="18" t="str">
+      <c r="H119" t="str">
         <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
         <v>Error</v>
       </c>
-      <c r="I119" s="18" t="str">
+      <c r="I119" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
         <v>owa,R_CL_EGT,R_CL_EGT_L.ttl,error</v>
       </c>
-      <c r="J119" s="18" t="str">
+      <c r="J119" t="str">
         <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
         <v>cwa,R_CL_EGT,R_CL_EGT_L.ttl,error</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B120" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
+      </c>
+      <c r="C120" t="s">
+        <v>76</v>
+      </c>
+      <c r="D120" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
+        <v>R_CL_EMV_A</v>
+      </c>
+      <c r="E120" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>R_CL_EMV_A.ttl</v>
+      </c>
+      <c r="F120" t="s">
+        <v>359</v>
+      </c>
+      <c r="G120" t="s">
+        <v>78</v>
+      </c>
+      <c r="H120" t="str">
+        <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
+        <v>Valid</v>
+      </c>
+      <c r="I120" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,R_CL_EMV,R_CL_EMV_A.ttl,valid</v>
+      </c>
+      <c r="J120" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,R_CL_EMV,R_CL_EMV_A.ttl,valid</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B121" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
+      </c>
+      <c r="C121" t="s">
+        <v>77</v>
+      </c>
+      <c r="D121" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
+        <v>R_CL_EMV_B</v>
+      </c>
+      <c r="E121" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>R_CL_EMV_B.ttl</v>
+      </c>
+      <c r="F121" t="s">
+        <v>360</v>
+      </c>
+      <c r="G121" t="s">
+        <v>78</v>
+      </c>
+      <c r="H121" t="str">
+        <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
+        <v>Valid</v>
+      </c>
+      <c r="I121" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,R_CL_EMV,R_CL_EMV_B.ttl,valid</v>
+      </c>
+      <c r="J121" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,R_CL_EMV,R_CL_EMV_B.ttl,valid</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B122" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
+      </c>
+      <c r="C122" t="s">
+        <v>79</v>
+      </c>
+      <c r="D122" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
+        <v>R_CL_EMV_C</v>
+      </c>
+      <c r="E122" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>R_CL_EMV_C.ttl</v>
+      </c>
+      <c r="F122" t="s">
+        <v>395</v>
+      </c>
+      <c r="G122" t="s">
+        <v>72</v>
+      </c>
+      <c r="H122" t="str">
+        <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
+        <v>Error</v>
+      </c>
+      <c r="I122" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,R_CL_EMV,R_CL_EMV_C.ttl,warning</v>
+      </c>
+      <c r="J122" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,R_CL_EMV,R_CL_EMV_C.ttl,error</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B123" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
+      </c>
+      <c r="C123" t="s">
+        <v>85</v>
+      </c>
+      <c r="D123" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
+        <v>R_CL_EMV_D</v>
+      </c>
+      <c r="E123" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>R_CL_EMV_D.ttl</v>
+      </c>
+      <c r="F123" t="s">
+        <v>400</v>
+      </c>
+      <c r="G123" t="s">
+        <v>73</v>
+      </c>
+      <c r="H123" t="str">
+        <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
+        <v>Error</v>
+      </c>
+      <c r="I123" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,R_CL_EMV,R_CL_EMV_D.ttl,error</v>
+      </c>
+      <c r="J123" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,R_CL_EMV,R_CL_EMV_D.ttl,error</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B124" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
+      </c>
+      <c r="C124" t="s">
+        <v>86</v>
+      </c>
+      <c r="D124" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
+        <v>R_CL_EMV_E</v>
+      </c>
+      <c r="E124" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>R_CL_EMV_E.ttl</v>
+      </c>
+      <c r="F124" t="s">
+        <v>396</v>
+      </c>
+      <c r="G124" t="s">
+        <v>78</v>
+      </c>
+      <c r="H124" t="str">
+        <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
+        <v>Valid</v>
+      </c>
+      <c r="I124" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,R_CL_EMV,R_CL_EMV_E.ttl,valid</v>
+      </c>
+      <c r="J124" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,R_CL_EMV,R_CL_EMV_E.ttl,valid</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B125" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
+      </c>
+      <c r="C125" t="s">
+        <v>87</v>
+      </c>
+      <c r="D125" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
+        <v>R_CL_EMV_F</v>
+      </c>
+      <c r="E125" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>R_CL_EMV_F.ttl</v>
+      </c>
+      <c r="F125" t="s">
+        <v>398</v>
+      </c>
+      <c r="G125" t="s">
+        <v>73</v>
+      </c>
+      <c r="H125" t="str">
+        <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
+        <v>Error</v>
+      </c>
+      <c r="I125" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,R_CL_EMV,R_CL_EMV_F.ttl,error</v>
+      </c>
+      <c r="J125" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,R_CL_EMV,R_CL_EMV_F.ttl,error</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B126" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
+      </c>
+      <c r="C126" t="s">
+        <v>367</v>
+      </c>
+      <c r="D126" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
+        <v>R_CL_EMV_G</v>
+      </c>
+      <c r="E126" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>R_CL_EMV_G.ttl</v>
+      </c>
+      <c r="F126" t="s">
+        <v>397</v>
+      </c>
+      <c r="G126" t="s">
+        <v>78</v>
+      </c>
+      <c r="H126" t="str">
+        <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
+        <v>Valid</v>
+      </c>
+      <c r="I126" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,R_CL_EMV,R_CL_EMV_G.ttl,valid</v>
+      </c>
+      <c r="J126" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,R_CL_EMV,R_CL_EMV_G.ttl,valid</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B127" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
+      </c>
+      <c r="C127" t="s">
+        <v>368</v>
+      </c>
+      <c r="D127" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
+        <v>R_CL_EMV_H</v>
+      </c>
+      <c r="E127" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>R_CL_EMV_H.ttl</v>
+      </c>
+      <c r="F127" t="s">
+        <v>399</v>
+      </c>
+      <c r="G127" t="s">
+        <v>73</v>
+      </c>
+      <c r="H127" t="str">
+        <f>IF(TabImp[[#This Row],[OWA Level]]="Valid","Valid","Error")</f>
+        <v>Error</v>
+      </c>
+      <c r="I127" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,R_CL_EMV,R_CL_EMV_H.ttl,error</v>
+      </c>
+      <c r="J127" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,R_CL_EMV,R_CL_EMV_H.ttl,error</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="D2:E127">
+    <cfRule type="duplicateValues" dxfId="3" priority="48"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G2:H254">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Valid"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:E119">
-    <cfRule type="duplicateValues" dxfId="3" priority="37"/>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H119" xr:uid="{88F4C713-6BF6-49A8-982F-7D1643817146}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H127" xr:uid="{88F4C713-6BF6-49A8-982F-7D1643817146}">
       <formula1>"Valid,Error,Warning"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8357,7 +8589,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8368,74 +8600,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" t="s">
         <v>348</v>
-      </c>
-      <c r="B2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B3" t="s">
         <v>354</v>
-      </c>
-      <c r="B3" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor modification on ontouml lib
</commit_message>
<xml_diff>
--- a/resources/OntoUML Rules.xlsx
+++ b/resources/OntoUML Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FavatoBarcelosPP\Dev\ontouml-validator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC85260C-F7D0-4DC4-B60C-CD1DC861A973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A29F04-0F1A-4A5F-93A7-9F48BC83AD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="405">
   <si>
     <t>Description</t>
   </si>
@@ -1057,9 +1057,6 @@
     <t>Every class decorated with a base sortal stereotype and the tagged value "order" set to "1" must have the tagged value "restrictedTo" set to an array containing one of the values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality" ].</t>
   </si>
   <si>
-    <t>Every class decorated with a non-sortal stereotype and the tagged value "order" set to "1" must have the tagged value "restrictedTo" set to an array containing one or more of the values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality" ].</t>
-  </si>
-  <si>
     <t>Every class decorated with a non-sortal stereotype must be abstract.</t>
   </si>
   <si>
@@ -1228,9 +1225,6 @@
     <t>ALX</t>
   </si>
   <si>
-    <t>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</t>
-  </si>
-  <si>
     <t>R_CL_ALX</t>
   </si>
   <si>
@@ -1244,6 +1238,18 @@
   </si>
   <si>
     <t>Every class decorated with a BASE SORTAL stereotype must specialize a unique class decorated with a ULTIMATE SORTAL stereotype .</t>
+  </si>
+  <si>
+    <t>Every class decorated with a NON-SORTAL stereotype and the tagged value "order" set to "1" must have the tagged value "restrictedTo" set to an array containing one or more of the values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality" ].</t>
+  </si>
+  <si>
+    <t>Every class decorated with a RIGID or SEMI-RIGID stereotype cannot specialize classes decorated with an ANTI-RIGID stereotype.</t>
+  </si>
+  <si>
+    <t>BLE</t>
+  </si>
+  <si>
+    <t>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1400,7 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1445,6 +1451,10 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1453,6 +1463,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1480,36 +1520,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1728,11 +1738,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}" name="TabRules" displayName="TabRules" ref="A1:E72" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:E72" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D72">
-    <sortCondition ref="A2:A72"/>
-    <sortCondition ref="D2:D72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}" name="TabRules" displayName="TabRules" ref="A1:E73" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:E73" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
+    <sortCondition ref="A2:A73"/>
+    <sortCondition ref="D2:D73"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F9D36F48-DD19-43E5-A1AB-8357F96419FF}" name="Group" dataDxfId="22"/>
@@ -2107,12 +2117,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G95" sqref="G95"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2140,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G1" t="s">
         <v>97</v>
@@ -2292,7 +2302,7 @@
         <v>R_CL_ZGT</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E8"/>
     </row>
@@ -2301,14 +2311,14 @@
         <v>1</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C9" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
         <v>R_CL_ALX</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="E9"/>
     </row>
@@ -2317,30 +2327,30 @@
         <v>1</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="C10" s="9" t="str">
+        <v>403</v>
+      </c>
+      <c r="C10" s="20" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_ASZ</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="E10"/>
+        <v>R_CL_BLE</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C11" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_YOK</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>341</v>
+        <v>R_CL_ASZ</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>401</v>
       </c>
       <c r="E11"/>
     </row>
@@ -2349,49 +2359,49 @@
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C12" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_QJC</v>
+        <v>R_CL_YOK</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>387</v>
+        <v>340</v>
       </c>
       <c r="E12"/>
-      <c r="G12" s="14" t="s">
-        <v>241</v>
-      </c>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C13" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_ZEF</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>4</v>
+        <v>R_CL_QJC</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>386</v>
       </c>
       <c r="E13"/>
+      <c r="G13" s="14" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C14" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_PSQ</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>5</v>
+        <v>R_CL_ZEF</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>4</v>
       </c>
       <c r="E14"/>
     </row>
@@ -2400,14 +2410,14 @@
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C15" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_SQU</v>
+        <v>R_CL_PSQ</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15"/>
     </row>
@@ -2416,14 +2426,14 @@
         <v>1</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="C16" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_XJZ</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>3</v>
+        <v>R_CL_SQU</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="E16"/>
     </row>
@@ -2432,14 +2442,14 @@
         <v>1</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C17" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_JOJ</v>
+        <v>R_CL_XJZ</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="E17"/>
     </row>
@@ -2448,14 +2458,14 @@
         <v>1</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C18" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_GJU</v>
+        <v>R_CL_JOJ</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E18"/>
     </row>
@@ -2464,14 +2474,14 @@
         <v>1</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C19" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_BWZ</v>
+        <v>R_CL_GJU</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E19"/>
     </row>
@@ -2480,14 +2490,14 @@
         <v>1</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C20" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_JMQ</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>14</v>
+        <v>R_CL_BWZ</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>2</v>
       </c>
       <c r="E20"/>
     </row>
@@ -2496,14 +2506,14 @@
         <v>1</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C21" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_EMV</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>9</v>
+        <v>R_CL_JMQ</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E21"/>
     </row>
@@ -2512,14 +2522,14 @@
         <v>1</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C22" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_QOV</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>349</v>
+        <v>R_CL_EMV</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="E22"/>
     </row>
@@ -2528,14 +2538,14 @@
         <v>1</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C23" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_JFW</v>
+        <v>R_CL_QOV</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>17</v>
+        <v>348</v>
       </c>
       <c r="E23"/>
     </row>
@@ -2544,14 +2554,14 @@
         <v>1</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C24" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_UTL</v>
+        <v>R_CL_JFW</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E24"/>
     </row>
@@ -2560,14 +2570,14 @@
         <v>1</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C25" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_VPE</v>
+        <v>R_CL_UTL</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E25"/>
     </row>
@@ -2576,14 +2586,14 @@
         <v>1</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C26" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_BFO</v>
+        <v>R_CL_VPE</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E26"/>
     </row>
@@ -2592,14 +2602,14 @@
         <v>1</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C27" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_VOQ</v>
+        <v>R_CL_BFO</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E27"/>
     </row>
@@ -2608,14 +2618,14 @@
         <v>1</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C28" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_GAZ</v>
+        <v>R_CL_VOQ</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E28"/>
     </row>
@@ -2624,14 +2634,14 @@
         <v>1</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C29" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_BQI</v>
+        <v>R_CL_GAZ</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E29"/>
     </row>
@@ -2640,14 +2650,14 @@
         <v>1</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="C30" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_UMC</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>95</v>
+        <v>R_CL_BQI</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="E30"/>
     </row>
@@ -2656,14 +2666,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="C31" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_OEV</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>20</v>
+        <v>R_CL_UMC</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="E31"/>
     </row>
@@ -2672,14 +2682,14 @@
         <v>1</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C32" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_EGT</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>368</v>
+        <v>R_CL_OEV</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="E32"/>
     </row>
@@ -2688,30 +2698,30 @@
         <v>1</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C33" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_CL_ANY</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>16</v>
+        <v>R_CL_EGT</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>367</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C34" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_XRS</v>
+        <v>R_CL_ANY</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E34"/>
     </row>
@@ -2720,14 +2730,14 @@
         <v>21</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C35" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_MDR</v>
+        <v>R_GE_XRS</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E35"/>
     </row>
@@ -2736,14 +2746,14 @@
         <v>21</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C36" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_BAK</v>
+        <v>R_GE_MDR</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E36"/>
     </row>
@@ -2752,14 +2762,14 @@
         <v>21</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C37" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_JLW</v>
+        <v>R_GE_BAK</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E37"/>
     </row>
@@ -2768,14 +2778,14 @@
         <v>21</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C38" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_VEZ</v>
+        <v>R_GE_JLW</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E38"/>
     </row>
@@ -2784,14 +2794,14 @@
         <v>21</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C39" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_IJM</v>
+        <v>R_GE_VEZ</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E39"/>
     </row>
@@ -2800,14 +2810,14 @@
         <v>21</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C40" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_UXR</v>
+        <v>R_GE_IJM</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E40"/>
     </row>
@@ -2816,14 +2826,14 @@
         <v>21</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C41" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_HGQ</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>401</v>
+        <v>R_GE_UXR</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="E41"/>
     </row>
@@ -2832,14 +2842,14 @@
         <v>21</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>399</v>
+        <v>280</v>
       </c>
       <c r="C42" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_KNF</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>400</v>
+        <v>R_GE_HGQ</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>399</v>
       </c>
       <c r="E42"/>
     </row>
@@ -2848,14 +2858,14 @@
         <v>21</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>281</v>
+        <v>397</v>
       </c>
       <c r="C43" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_EPG</v>
+        <v>R_GE_KNF</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>333</v>
+        <v>398</v>
       </c>
       <c r="E43"/>
     </row>
@@ -2864,14 +2874,14 @@
         <v>21</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C44" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_MXI</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>350</v>
+        <v>R_GE_EPG</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>333</v>
       </c>
       <c r="E44"/>
     </row>
@@ -2880,30 +2890,30 @@
         <v>21</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C45" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GE_HPZ</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>27</v>
+        <v>R_GE_MXI</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>349</v>
       </c>
       <c r="E45"/>
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C46" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_LHD</v>
+        <v>R_GE_HPZ</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E46"/>
     </row>
@@ -2912,14 +2922,14 @@
         <v>53</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C47" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_PQP</v>
+        <v>R_GS_LHD</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E47"/>
     </row>
@@ -2928,14 +2938,14 @@
         <v>53</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C48" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_UTW</v>
+        <v>R_GS_PQP</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E48"/>
     </row>
@@ -2944,14 +2954,14 @@
         <v>53</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C49" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_YKW</v>
+        <v>R_GS_UTW</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E49"/>
     </row>
@@ -2960,14 +2970,14 @@
         <v>53</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C50" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_XXB</v>
+        <v>R_GS_YKW</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E50"/>
     </row>
@@ -2976,30 +2986,30 @@
         <v>53</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C51" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_GS_ZMQ</v>
+        <v>R_GS_XXB</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E51"/>
     </row>
     <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C52" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_PR_BWY</v>
+        <v>R_GS_ZMQ</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E52"/>
     </row>
@@ -3008,30 +3018,30 @@
         <v>50</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C53" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_PR_LCI</v>
+        <v>R_PR_BWY</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E53"/>
     </row>
     <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C54" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_AZO</v>
+        <v>R_PR_LCI</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E54"/>
     </row>
@@ -3040,14 +3050,14 @@
         <v>30</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C55" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_ECP</v>
+        <v>R_RE_AZO</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E55"/>
     </row>
@@ -3056,14 +3066,14 @@
         <v>30</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C56" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_FIX</v>
+        <v>R_RE_ECP</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E56"/>
     </row>
@@ -3072,14 +3082,14 @@
         <v>30</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C57" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_HGG</v>
+        <v>R_RE_FIX</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E57"/>
     </row>
@@ -3088,14 +3098,14 @@
         <v>30</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C58" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_VDQ</v>
+        <v>R_RE_HGG</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E58"/>
     </row>
@@ -3104,14 +3114,14 @@
         <v>30</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C59" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_VMI</v>
+        <v>R_RE_VDQ</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E59"/>
     </row>
@@ -3120,14 +3130,14 @@
         <v>30</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C60" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_ALR</v>
+        <v>R_RE_VMI</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E60"/>
     </row>
@@ -3136,14 +3146,14 @@
         <v>30</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C61" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_SEI</v>
+        <v>R_RE_ALR</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E61"/>
     </row>
@@ -3152,14 +3162,14 @@
         <v>30</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C62" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_EAQ</v>
+        <v>R_RE_SEI</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E62"/>
     </row>
@@ -3168,14 +3178,14 @@
         <v>30</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C63" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_CDJ</v>
+        <v>R_RE_EAQ</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E63"/>
     </row>
@@ -3184,14 +3194,14 @@
         <v>30</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C64" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_RON</v>
+        <v>R_RE_CDJ</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E64"/>
     </row>
@@ -3200,14 +3210,14 @@
         <v>30</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C65" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_KZC</v>
+        <v>R_RE_RON</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E65"/>
     </row>
@@ -3216,14 +3226,14 @@
         <v>30</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C66" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_NTY</v>
+        <v>R_RE_KZC</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E66"/>
     </row>
@@ -3232,14 +3242,14 @@
         <v>30</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C67" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_UCH</v>
+        <v>R_RE_NTY</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E67"/>
     </row>
@@ -3248,14 +3258,14 @@
         <v>30</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C68" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_LQF</v>
+        <v>R_RE_UCH</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E68"/>
     </row>
@@ -3264,14 +3274,14 @@
         <v>30</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C69" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_GZN</v>
+        <v>R_RE_LQF</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E69"/>
     </row>
@@ -3280,14 +3290,14 @@
         <v>30</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C70" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_KPG</v>
+        <v>R_RE_GZN</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E70"/>
     </row>
@@ -3296,14 +3306,14 @@
         <v>30</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C71" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
-        <v>R_RE_GZF</v>
+        <v>R_RE_KPG</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E71"/>
     </row>
@@ -3312,42 +3322,58 @@
         <v>30</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C72" s="9" t="str">
         <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
+        <v>R_RE_GZF</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72"/>
+    </row>
+    <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C73" s="9" t="str">
+        <f>"R_"&amp;VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[ID]]</f>
         <v>R_RE_JND</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="D73" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E72"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
+      <c r="E73"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D75" s="11"/>
-      <c r="E75" s="6"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D76" s="6"/>
+      <c r="D76" s="11"/>
       <c r="E76" s="6"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E78" s="11"/>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B72">
-    <cfRule type="duplicateValues" dxfId="6" priority="43"/>
+  <conditionalFormatting sqref="B2:B73">
+    <cfRule type="duplicateValues" dxfId="2" priority="49"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C72">
-    <cfRule type="duplicateValues" dxfId="5" priority="45"/>
+  <conditionalFormatting sqref="C2:C73">
+    <cfRule type="duplicateValues" dxfId="1" priority="51"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:E72">
-    <cfRule type="duplicateValues" dxfId="4" priority="47"/>
+  <conditionalFormatting sqref="D2:E73">
+    <cfRule type="duplicateValues" dxfId="0" priority="53"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3366,8 +3392,8 @@
   <dimension ref="A1:M184"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7584,7 +7610,7 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B100" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7602,7 +7628,7 @@
         <v>R_CL_QJC_A.ttl</v>
       </c>
       <c r="F100" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G100" t="s">
         <v>75</v>
@@ -7622,7 +7648,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B101" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7640,7 +7666,7 @@
         <v>R_CL_QJC_B.ttl</v>
       </c>
       <c r="F101" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G101" t="s">
         <v>75</v>
@@ -7660,7 +7686,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B102" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7678,7 +7704,7 @@
         <v>R_CL_QJC_C.ttl</v>
       </c>
       <c r="F102" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G102" t="s">
         <v>75</v>
@@ -7701,7 +7727,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B103" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7719,7 +7745,7 @@
         <v>R_CL_QJC_D.ttl</v>
       </c>
       <c r="F103" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G103" t="s">
         <v>75</v>
@@ -7737,12 +7763,12 @@
         <v>cwa,R_CL_QJC,R_CL_QJC_D.ttl,valid</v>
       </c>
       <c r="K103" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B104" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7760,7 +7786,7 @@
         <v>R_CL_QJC_E.ttl</v>
       </c>
       <c r="F104" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G104" t="s">
         <v>75</v>
@@ -7783,7 +7809,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B105" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7801,7 +7827,7 @@
         <v>R_CL_QJC_F.ttl</v>
       </c>
       <c r="F105" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G105" t="s">
         <v>70</v>
@@ -7819,19 +7845,19 @@
         <v>cwa,R_CL_QJC,R_CL_QJC_F.ttl,error</v>
       </c>
       <c r="K105" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B106" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C106" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D106" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -7842,7 +7868,7 @@
         <v>R_CL_QJC_G.ttl</v>
       </c>
       <c r="F106" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G106" t="s">
         <v>75</v>
@@ -7860,19 +7886,19 @@
         <v>cwa,R_CL_QJC,R_CL_QJC_G.ttl,valid</v>
       </c>
       <c r="K106" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B107" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>Each class with one of the following stereotypes must exclusively map to the corresponding 'restrictedTo' value: collective to collective, event to event, kind to functional-complex, quality to quality, quantity to quantity, relator to relator, situation to situation, abstract to abstract, enumeration to abstract, and datatype to abstract.</v>
       </c>
       <c r="C107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D107" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -7883,7 +7909,7 @@
         <v>R_CL_QJC_H.ttl</v>
       </c>
       <c r="F107" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G107" t="s">
         <v>70</v>
@@ -7901,12 +7927,12 @@
         <v>cwa,R_CL_QJC,R_CL_QJC_H.ttl,error</v>
       </c>
       <c r="K107" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B108" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7924,7 +7950,7 @@
         <v>R_CL_EGT_A.ttl</v>
       </c>
       <c r="F108" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G108" t="s">
         <v>75</v>
@@ -7944,7 +7970,7 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B109" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -7962,7 +7988,7 @@
         <v>R_CL_EGT_B.ttl</v>
       </c>
       <c r="F109" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G109" t="s">
         <v>70</v>
@@ -7980,12 +8006,12 @@
         <v>cwa,R_CL_EGT,R_CL_EGT_B.ttl,error</v>
       </c>
       <c r="K109" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B110" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8003,7 +8029,7 @@
         <v>R_CL_EGT_C.ttl</v>
       </c>
       <c r="F110" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G110" t="s">
         <v>75</v>
@@ -8023,7 +8049,7 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B111" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8041,7 +8067,7 @@
         <v>R_CL_EGT_D.ttl</v>
       </c>
       <c r="F111" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G111" t="s">
         <v>70</v>
@@ -8059,12 +8085,12 @@
         <v>cwa,R_CL_EGT,R_CL_EGT_D.ttl,error</v>
       </c>
       <c r="K111" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B112" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8082,7 +8108,7 @@
         <v>R_CL_EGT_E.ttl</v>
       </c>
       <c r="F112" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G112" t="s">
         <v>75</v>
@@ -8102,7 +8128,7 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B113" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8120,7 +8146,7 @@
         <v>R_CL_EGT_F.ttl</v>
       </c>
       <c r="F113" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G113" t="s">
         <v>70</v>
@@ -8138,19 +8164,19 @@
         <v>cwa,R_CL_EGT,R_CL_EGT_F.ttl,error</v>
       </c>
       <c r="K113" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B114" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C114" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D114" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -8161,7 +8187,7 @@
         <v>R_CL_EGT_G.ttl</v>
       </c>
       <c r="F114" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G114" t="s">
         <v>70</v>
@@ -8179,19 +8205,19 @@
         <v>cwa,R_CL_EGT,R_CL_EGT_G.ttl,error</v>
       </c>
       <c r="K114" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B115" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C115" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D115" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -8202,7 +8228,7 @@
         <v>R_CL_EGT_H.ttl</v>
       </c>
       <c r="F115" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G115" t="s">
         <v>75</v>
@@ -8222,14 +8248,14 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B116" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C116" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D116" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -8240,7 +8266,7 @@
         <v>R_CL_EGT_I.ttl</v>
       </c>
       <c r="F116" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G116" t="s">
         <v>70</v>
@@ -8258,19 +8284,19 @@
         <v>cwa,R_CL_EGT,R_CL_EGT_I.ttl,error</v>
       </c>
       <c r="K116" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B117" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C117" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D117" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -8281,7 +8307,7 @@
         <v>R_CL_EGT_J.ttl</v>
       </c>
       <c r="F117" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G117" t="s">
         <v>70</v>
@@ -8299,19 +8325,19 @@
         <v>cwa,R_CL_EGT,R_CL_EGT_J.ttl,error</v>
       </c>
       <c r="K117" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B118" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C118" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D118" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -8322,7 +8348,7 @@
         <v>R_CL_EGT_K.ttl</v>
       </c>
       <c r="F118" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G118" t="s">
         <v>75</v>
@@ -8342,14 +8368,14 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B119" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>No class can have one of its subclasses as its superclasses.</v>
       </c>
       <c r="C119" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D119" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -8360,7 +8386,7 @@
         <v>R_CL_EGT_L.ttl</v>
       </c>
       <c r="F119" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G119" t="s">
         <v>70</v>
@@ -8380,7 +8406,7 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B120" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8398,7 +8424,7 @@
         <v>R_CL_EMV_A.ttl</v>
       </c>
       <c r="F120" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G120" t="s">
         <v>75</v>
@@ -8418,7 +8444,7 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B121" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8436,7 +8462,7 @@
         <v>R_CL_EMV_B.ttl</v>
       </c>
       <c r="F121" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G121" t="s">
         <v>75</v>
@@ -8456,7 +8482,7 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B122" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8474,7 +8500,7 @@
         <v>R_CL_EMV_C.ttl</v>
       </c>
       <c r="F122" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G122" t="s">
         <v>69</v>
@@ -8494,7 +8520,7 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B123" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8512,7 +8538,7 @@
         <v>R_CL_EMV_D.ttl</v>
       </c>
       <c r="F123" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G123" t="s">
         <v>70</v>
@@ -8532,7 +8558,7 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B124" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8550,7 +8576,7 @@
         <v>R_CL_EMV_E.ttl</v>
       </c>
       <c r="F124" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G124" t="s">
         <v>75</v>
@@ -8570,7 +8596,7 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B125" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
@@ -8588,7 +8614,7 @@
         <v>R_CL_EMV_F.ttl</v>
       </c>
       <c r="F125" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G125" t="s">
         <v>70</v>
@@ -8608,14 +8634,14 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B126" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
       </c>
       <c r="C126" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D126" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -8626,7 +8652,7 @@
         <v>R_CL_EMV_G.ttl</v>
       </c>
       <c r="F126" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G126" t="s">
         <v>75</v>
@@ -8646,14 +8672,14 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B127" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must have the tagged value "restrictedTo" set to one or more values in the list [ "functional-complex", "collective", "quantity", "relator", "intrinsic-mode", "extrinsic-mode", "quality", "event", "situation", "abstract", "type" ].</v>
       </c>
       <c r="C127" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D127" s="12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;"_"&amp;TabImp[[#This Row],[Situation]]</f>
@@ -8664,7 +8690,7 @@
         <v>R_CL_EMV_H.ttl</v>
       </c>
       <c r="F127" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G127" t="s">
         <v>70</v>
@@ -8684,11 +8710,11 @@
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B128" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C128" t="s">
         <v>209</v>
@@ -8722,11 +8748,11 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B129" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C129" t="s">
         <v>210</v>
@@ -8760,11 +8786,11 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B130" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C130" t="s">
         <v>211</v>
@@ -8798,11 +8824,11 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B131" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C131" t="s">
         <v>212</v>
@@ -8836,11 +8862,11 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B132" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C132" t="s">
         <v>213</v>
@@ -8874,11 +8900,11 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B133" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C133" t="s">
         <v>214</v>
@@ -8912,11 +8938,11 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B134" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C134" t="s">
         <v>215</v>
@@ -8950,11 +8976,11 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B135" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C135" t="s">
         <v>216</v>
@@ -8988,11 +9014,11 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B136" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C136" t="s">
         <v>217</v>
@@ -9026,11 +9052,11 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B137" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C137" t="s">
         <v>179</v>
@@ -9064,11 +9090,11 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B138" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C138" t="s">
         <v>180</v>
@@ -9102,11 +9128,11 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B139" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C139" t="s">
         <v>181</v>
@@ -9140,11 +9166,11 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B140" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C140" t="s">
         <v>182</v>
@@ -9178,11 +9204,11 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B141" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C141" t="s">
         <v>183</v>
@@ -9216,11 +9242,11 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B142" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C142" t="s">
         <v>184</v>
@@ -9254,11 +9280,11 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B143" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C143" t="s">
         <v>185</v>
@@ -9292,11 +9318,11 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B144" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C144" t="s">
         <v>186</v>
@@ -9330,11 +9356,11 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B145" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C145" t="s">
         <v>187</v>
@@ -9368,11 +9394,11 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B146" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C146" t="s">
         <v>188</v>
@@ -9406,11 +9432,11 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B147" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C147" t="s">
         <v>218</v>
@@ -9444,11 +9470,11 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B148" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C148" t="s">
         <v>219</v>
@@ -9482,11 +9508,11 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B149" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C149" t="s">
         <v>220</v>
@@ -9520,11 +9546,11 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B150" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C150" t="s">
         <v>221</v>
@@ -9558,11 +9584,11 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B151" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C151" t="s">
         <v>222</v>
@@ -9596,11 +9622,11 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B152" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C152" t="s">
         <v>223</v>
@@ -9634,11 +9660,11 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B153" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C153" t="s">
         <v>224</v>
@@ -9672,11 +9698,11 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B154" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C154" t="s">
         <v>225</v>
@@ -9710,11 +9736,11 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B155" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C155" t="s">
         <v>226</v>
@@ -9748,11 +9774,11 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B156" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C156" t="s">
         <v>189</v>
@@ -9786,11 +9812,11 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B157" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C157" t="s">
         <v>190</v>
@@ -9824,11 +9850,11 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B158" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C158" t="s">
         <v>191</v>
@@ -9862,11 +9888,11 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B159" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C159" t="s">
         <v>192</v>
@@ -9900,11 +9926,11 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B160" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C160" t="s">
         <v>193</v>
@@ -9938,11 +9964,11 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B161" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C161" t="s">
         <v>194</v>
@@ -9976,11 +10002,11 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B162" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C162" t="s">
         <v>195</v>
@@ -10014,11 +10040,11 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B163" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C163" t="s">
         <v>196</v>
@@ -10052,11 +10078,11 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B164" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C164" t="s">
         <v>197</v>
@@ -10090,11 +10116,11 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B165" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C165" t="s">
         <v>198</v>
@@ -10128,11 +10154,11 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B166" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C166" t="s">
         <v>227</v>
@@ -10166,11 +10192,11 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B167" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C167" t="s">
         <v>228</v>
@@ -10204,11 +10230,11 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B168" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C168" t="s">
         <v>229</v>
@@ -10242,11 +10268,11 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B169" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C169" t="s">
         <v>230</v>
@@ -10280,11 +10306,11 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B170" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C170" t="s">
         <v>231</v>
@@ -10318,11 +10344,11 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B171" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C171" t="s">
         <v>232</v>
@@ -10356,11 +10382,11 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B172" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C172" t="s">
         <v>233</v>
@@ -10394,11 +10420,11 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B173" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C173" t="s">
         <v>234</v>
@@ -10432,11 +10458,11 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B174" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C174" t="s">
         <v>235</v>
@@ -10470,11 +10496,11 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B175" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C175" t="s">
         <v>199</v>
@@ -10508,11 +10534,11 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B176" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C176" t="s">
         <v>200</v>
@@ -10546,11 +10572,11 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B177" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C177" t="s">
         <v>201</v>
@@ -10584,11 +10610,11 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B178" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C178" t="s">
         <v>202</v>
@@ -10622,11 +10648,11 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B179" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C179" t="s">
         <v>203</v>
@@ -10660,11 +10686,11 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B180" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C180" t="s">
         <v>204</v>
@@ -10698,11 +10724,11 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B181" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C181" t="s">
         <v>205</v>
@@ -10736,11 +10762,11 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B182" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C182" t="s">
         <v>206</v>
@@ -10774,11 +10800,11 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B183" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C183" t="s">
         <v>207</v>
@@ -10812,11 +10838,11 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B184" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[Rule Code]:[Description]],2,FALSE)</f>
-        <v>Every class decorated with a ULTIMATE SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
+        <v>Every class decorated with a ULTIMATE SORTAL or a NON-SORTAL stereotype cannot specialize classes decorated with a SORTAL or an ABSTRACT stereotype.</v>
       </c>
       <c r="C184" t="s">
         <v>208</v>
@@ -10851,16 +10877,16 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="D2:E184">
-    <cfRule type="duplicateValues" dxfId="3" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:H254">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Valid"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10893,7 +10919,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B1" t="s">
         <v>329</v>
@@ -10901,18 +10927,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B2" t="s">
         <v>342</v>
-      </c>
-      <c r="B2" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -10933,18 +10959,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>